<commit_message>
Updated with latest SOP
</commit_message>
<xml_diff>
--- a/sop_linkage_2025/Master SOP 2025.xlsx
+++ b/sop_linkage_2025/Master SOP 2025.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishi/codeBase/CNS/info_vis_client_projects/sop_linkage_2025/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED5CFC-1EFB-DF4A-80ED-2807698C9D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="2025-Master SOP" sheetId="1" r:id="rId4"/>
+    <sheet name="2025-Master SOP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="116">
   <si>
     <t>Master SOPs</t>
   </si>
@@ -307,9 +316,6 @@
     <t>10.5281/zenodo.6703107</t>
   </si>
   <si>
-    <t>Mapping Functional Tissue Unit Illustrations to ASCT+B Tables</t>
-  </si>
-  <si>
     <t>https://zenodo.org/doi/10.5281/zenodo.5748154</t>
   </si>
   <si>
@@ -356,57 +362,69 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41556-021-00788-6</t>
+  </si>
+  <si>
+    <t>Authoring Crosswalk Tables Between Functional Tissue Unit Illustrations and ASCT+B Tables</t>
+  </si>
+  <si>
+    <t>Version v2.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF467886"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,58 +432,50 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -655,27 +665,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="86.5"/>
-    <col customWidth="1" min="2" max="2" width="73.5"/>
-    <col customWidth="1" min="3" max="3" width="111.75"/>
-    <col customWidth="1" min="4" max="4" width="24.75"/>
-    <col customWidth="1" min="5" max="5" width="13.63"/>
+    <col min="1" max="1" width="86.5" customWidth="1"/>
+    <col min="2" max="2" width="88" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,77 +707,77 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -772,25 +787,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -800,12 +815,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -815,12 +830,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -830,12 +845,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -845,14 +860,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -862,12 +877,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -877,12 +892,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -892,38 +907,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -933,12 +948,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -948,12 +963,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -963,12 +978,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -978,12 +993,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -993,27 +1008,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1023,14 +1038,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1040,12 +1055,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="2"/>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1055,14 +1070,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1072,27 +1087,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1102,14 +1117,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1119,14 +1134,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1136,14 +1151,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1153,153 +1168,153 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2"/>
-      <c r="B33" s="1" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2"/>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="8" t="s">
+      <c r="D39" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" location="heading=h.lpsf90jpnlzf" ref="C3"/>
-    <hyperlink r:id="rId3" ref="C4"/>
-    <hyperlink r:id="rId4" location="heading=h.lpsf90jpnlzf" ref="C5"/>
-    <hyperlink r:id="rId5" ref="C6"/>
-    <hyperlink r:id="rId6" ref="C7"/>
-    <hyperlink r:id="rId7" ref="C8"/>
-    <hyperlink r:id="rId8" ref="C9"/>
-    <hyperlink r:id="rId9" ref="C10"/>
-    <hyperlink r:id="rId10" ref="C11"/>
-    <hyperlink r:id="rId11" ref="C12"/>
-    <hyperlink r:id="rId12" ref="C13"/>
-    <hyperlink r:id="rId13" ref="C14"/>
-    <hyperlink r:id="rId14" ref="C15"/>
-    <hyperlink r:id="rId15" ref="C16"/>
-    <hyperlink r:id="rId16" ref="C17"/>
-    <hyperlink r:id="rId17" ref="C18"/>
-    <hyperlink r:id="rId18" ref="C19"/>
-    <hyperlink r:id="rId19" ref="C20"/>
-    <hyperlink r:id="rId20" ref="C21"/>
-    <hyperlink r:id="rId21" ref="C22"/>
-    <hyperlink r:id="rId22" location="heading=h.6ys5lo962o6b" ref="C23"/>
-    <hyperlink r:id="rId23" ref="C24"/>
-    <hyperlink r:id="rId24" ref="C25"/>
-    <hyperlink r:id="rId25" ref="C26"/>
-    <hyperlink r:id="rId26" ref="C27"/>
-    <hyperlink r:id="rId27" location="heading=h.6ys5lo962o6b" ref="C28"/>
-    <hyperlink r:id="rId28" ref="C29"/>
-    <hyperlink r:id="rId29" ref="C30"/>
-    <hyperlink r:id="rId30" ref="C31"/>
-    <hyperlink r:id="rId31" ref="C32"/>
-    <hyperlink r:id="rId32" ref="C33"/>
-    <hyperlink r:id="rId33" ref="C34"/>
-    <hyperlink r:id="rId34" location=".Y9R0knbMJmM" ref="C35"/>
-    <hyperlink r:id="rId35" location="heading=h.6ys5lo962o6b" ref="C36"/>
-    <hyperlink r:id="rId36" ref="C37"/>
-    <hyperlink r:id="rId37" ref="C38"/>
-    <hyperlink r:id="rId38" ref="C39"/>
-    <hyperlink r:id="rId39" ref="D39"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" location="heading=h.lpsf90jpnlzf" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" location="heading=h.lpsf90jpnlzf" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C23" r:id="rId22" location="heading=h.6ys5lo962o6b" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" location="heading=h.6ys5lo962o6b" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" location=".Y9R0knbMJmM" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" location="heading=h.6ys5lo962o6b" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D39" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
   </hyperlinks>
-  <drawing r:id="rId40"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>